<commit_message>
Modified automation to update test result
</commit_message>
<xml_diff>
--- a/EcoPower_Logistics/CMPG323 EcoPower Logistics Data.xlsx
+++ b/EcoPower_Logistics/CMPG323 EcoPower Logistics Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nttlimited-my.sharepoint.com/personal/jacqui_muller_dimensiondata_com/Documents/NWU/2023 CMPG323/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\nwuuser\documents\uipath\cmpg323-project4-36787426\ecopower_logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5546F926-6C85-4EAE-890A-D0833008B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B224C2EE-D72C-413C-83C8-0FBC3DD6E173}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020BFFD2-79F0-4B02-9FFD-1B6579BB24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="1560" windowWidth="20220" windowHeight="6510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1951,7 +1951,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
writing to excel file working
</commit_message>
<xml_diff>
--- a/EcoPower_Logistics/CMPG323 EcoPower Logistics Data.xlsx
+++ b/EcoPower_Logistics/CMPG323 EcoPower Logistics Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\nwuuser\documents\uipath\cmpg323-project4-36787426\ecopower_logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NWUUSER\Documents\UiPath\CMPG323-Project4-36787426\EcoPower_Logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020BFFD2-79F0-4B02-9FFD-1B6579BB24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4EB39F-C94E-4203-B617-53829B557499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="1560" windowWidth="20220" windowHeight="6510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="270" yWindow="1560" windowWidth="20220" windowHeight="6510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -730,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +779,9 @@
       <c r="E2">
         <v>5723177115</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -796,6 +799,9 @@
       <c r="E3">
         <v>9041993848</v>
       </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -813,6 +819,9 @@
       <c r="E4">
         <v>3738283528</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -830,6 +839,9 @@
       <c r="E5">
         <v>6447102299</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -847,6 +859,9 @@
       <c r="E6">
         <v>1878764468</v>
       </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -864,6 +879,9 @@
       <c r="E7">
         <v>9666552669</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -881,6 +899,9 @@
       <c r="E8">
         <v>2384982848</v>
       </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -898,6 +919,9 @@
       <c r="E9">
         <v>8945409882</v>
       </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -915,6 +939,9 @@
       <c r="E10">
         <v>1320602595</v>
       </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -932,6 +959,9 @@
       <c r="E11">
         <v>7968612324</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -949,6 +979,9 @@
       <c r="E12">
         <v>1578247192</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -966,6 +999,9 @@
       <c r="E13">
         <v>7425817353</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -982,6 +1018,14 @@
       </c>
       <c r="E14">
         <v>5815761997</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +1994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>